<commit_message>
Fix data to new version refs #638
</commit_message>
<xml_diff>
--- a/contents/office2013/excel/03/population.xlsx
+++ b/contents/office2013/excel/03/population.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\tmu\21_情報教育\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="975" yWindow="870" windowWidth="14955" windowHeight="11760"/>
   </bookViews>
@@ -662,11 +667,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="182" formatCode="##,###,###,##0.0;&quot;-&quot;#,###,###,##0.0"/>
+    <numFmt numFmtId="176" formatCode="##,###,###,##0.0;&quot;-&quot;#,###,###,##0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -1077,10 +1082,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1093,6 +1098,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1430,7 +1438,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1472,7 +1480,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1507,7 +1515,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1718,11 +1726,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.25" customWidth="1"/>
     <col min="2" max="3" width="11.875" customWidth="1"/>
@@ -1730,13 +1736,13 @@
     <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.25" thickBot="1"/>
-    <row r="3" spans="1:9" ht="16.5" thickBot="1">
+    <row r="2" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>101</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1794,7 +1800,7 @@
         <v>71.8</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1823,7 +1829,7 @@
         <v>149.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>90.7</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1881,7 +1887,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1910,7 +1916,7 @@
         <v>98.6</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1939,7 +1945,7 @@
         <v>130.4</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1968,7 +1974,7 @@
         <v>151.69999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1997,7 +2003,7 @@
         <v>488.1</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -2026,7 +2032,7 @@
         <v>314.7</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2055,7 +2061,7 @@
         <v>318.10000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2084,7 +2090,7 @@
         <v>1857.7</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -2113,7 +2119,7 @@
         <v>1174.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -2142,7 +2148,7 @@
         <v>5750.7</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -2171,7 +2177,7 @@
         <v>3639.1</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -2200,7 +2206,7 @@
         <v>193.2</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -2229,7 +2235,7 @@
         <v>261.7</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -2258,7 +2264,7 @@
         <v>280.5</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -2287,7 +2293,7 @@
         <v>196.1</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -2316,7 +2322,7 @@
         <v>198.1</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -2345,7 +2351,7 @@
         <v>161.9</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -2374,7 +2380,7 @@
         <v>198.4</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -2403,7 +2409,7 @@
         <v>487.5</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -2432,7 +2438,7 @@
         <v>1404.9</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -2461,7 +2467,7 @@
         <v>323.2</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -2490,7 +2496,7 @@
         <v>343.6</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -2519,7 +2525,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -2548,7 +2554,7 @@
         <v>4654.6000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -2577,7 +2583,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -2606,7 +2612,7 @@
         <v>385.1</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -2635,7 +2641,7 @@
         <v>219.2</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -2664,7 +2670,7 @@
         <v>173.1</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -2693,7 +2699,7 @@
         <v>110.7</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -2722,7 +2728,7 @@
         <v>275.2</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -2751,7 +2757,7 @@
         <v>339.3</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -2780,7 +2786,7 @@
         <v>244.2</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -2809,7 +2815,7 @@
         <v>195.4</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -2838,7 +2844,7 @@
         <v>539.5</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -2867,7 +2873,7 @@
         <v>258.5</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -2896,7 +2902,7 @@
         <v>112.1</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -2925,7 +2931,7 @@
         <v>1014.8</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -2954,7 +2960,7 @@
         <v>355.1</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -2983,7 +2989,7 @@
         <v>361.1</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -3012,7 +3018,7 @@
         <v>248.8</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <v>44</v>
       </c>
@@ -3041,7 +3047,7 @@
         <v>190.8</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -3070,7 +3076,7 @@
         <v>149.1</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <v>46</v>
       </c>
@@ -3099,7 +3105,7 @@
         <v>190.8</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="14.25" thickBot="1">
+    <row r="50" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>47</v>
       </c>
@@ -3143,7 +3149,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.78700000000000003" right="0.78700000000000003" top="0.98399999999999999" bottom="0.98399999999999999" header="0.51200000000000001" footer="0.51200000000000001"/>
@@ -3157,7 +3163,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.78700000000000003" right="0.78700000000000003" top="0.98399999999999999" bottom="0.98399999999999999" header="0.51200000000000001" footer="0.51200000000000001"/>

</xml_diff>